<commit_message>
Byttet til Native Client og LOCALHOST for enklere testing.
</commit_message>
<xml_diff>
--- a/GBD/Dokumenter/Endringer/Endringsønsker GBD - møte i faggruppen 10  mars 2016.xlsx
+++ b/GBD/Dokumenter/Endringer/Endringsønsker GBD - møte i faggruppen 10  mars 2016.xlsx
@@ -26,7 +26,7 @@
     <author>mrekdal</author>
   </authors>
   <commentList>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Skjema</t>
   </si>
@@ -172,9 +172,6 @@
     <t>Kontakt</t>
   </si>
   <si>
-    <t>Ferdig</t>
-  </si>
-  <si>
     <t>Kjell</t>
   </si>
   <si>
@@ -212,15 +209,31 @@
   </si>
   <si>
     <t>Einar</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -275,20 +288,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,329 +607,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="5.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="5" width="45.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="118.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="6.28515625" style="2" customWidth="1"/>
+    <col min="2" max="4" width="5.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2"/>
+    <col min="6" max="6" width="45.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="118.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G16" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D17" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="F17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D21" s="2">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="2">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C13" s="2">
+      <c r="F21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D22" s="2">
         <v>2</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="F22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D23" s="2">
         <v>2</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="2">
-        <v>2</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="2">
-        <v>2</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="2">
-        <v>2</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="2">
-        <f>SUM(C2:C20)</f>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D24" s="2">
+        <f>SUM(D2:D20)</f>
         <v>38.350000000000009</v>
       </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E31" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -948,16 +990,7 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Dokument for prosjektområde" ma:contentTypeID="0x010100CC9DFD08886E394E85873067B5CDD6A6" ma:contentTypeVersion="" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="6e194af714babb3629da6bfe1015a9b5" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Dokument for prosjektområde" ma:contentTypeID="0x010100CC9DFD08886E394E85873067B5CDD6A6" ma:contentTypeVersion="" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="6e194af714babb3629da6bfe1015a9b5" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128bd3d77d9d60b6dd2504be0b3c674b" ns2:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="$ListId:Project Documents;">
 <xsd:import namespace="$ListId:Project Documents;"/>
 <xsd:element name="properties">
@@ -1112,18 +1145,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><Status xmlns="$ListId:Project Documents;">Kladd</Status><Links xmlns="$ListId:Project Documents;" xsi:nil="true"/><Owner xmlns="$ListId:Project Documents;"><UserInfo><DisplayName></DisplayName><AccountId xsi:nil="true"></AccountId><AccountType/></UserInfo></Owner></documentManagement></p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1197736-FF03-45C6-8605-10A18C4B5004}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19BAB7FA-C4A9-454E-A922-9A58114BB5AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1141,6 +1175,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1197736-FF03-45C6-8605-10A18C4B5004}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B62A453-805D-42C2-9D14-387D854EA417}">
   <ds:schemaRefs>

</xml_diff>